<commit_message>
Files and Folders Redistribution
</commit_message>
<xml_diff>
--- a/PIP-Backlog.xlsx
+++ b/PIP-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\PIP-University-Administration-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9DBDC8-647F-450A-BD02-29837A8BABD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6569D1B-A193-44D2-B395-89D9CBEA76FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18450" windowHeight="11020" xr2:uid="{59053253-4EAC-46A3-8F35-147C6248C68F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>PIP Sprint</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>Add University's details</t>
+  </si>
+  <si>
+    <t>Create EER Diagram</t>
+  </si>
+  <si>
+    <t>On-Schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">early </t>
+  </si>
+  <si>
+    <t>On Time</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -344,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,6 +416,21 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -414,49 +444,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -785,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EF25C4-0706-4711-8224-01EE9F63F796}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,26 +815,30 @@
     <col min="2" max="2" width="22.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="29"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -826,15 +848,18 @@
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+      <c r="F3" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -843,90 +868,108 @@
       <c r="C4" s="11">
         <v>44442</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="32">
         <v>44442</v>
       </c>
       <c r="E4" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="16"/>
+      <c r="F4" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="21"/>
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="11">
         <v>44442</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="32">
         <v>44442</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="16"/>
+      <c r="F5" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="11">
         <v>44442</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="32">
         <v>44442</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
+      <c r="F6" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="11">
         <v>44442</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="32">
         <v>44442</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
+      <c r="F7" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="11">
         <v>44442</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="32">
         <v>44442</v>
       </c>
       <c r="E8" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="16"/>
+      <c r="F8" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="21"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="11">
         <v>44442</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="32">
         <v>44442</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+      <c r="F9" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -935,201 +978,278 @@
       <c r="C10" s="13">
         <v>44449</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="33">
         <v>44442</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
+      <c r="F10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="22"/>
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="13">
         <v>44449</v>
       </c>
-      <c r="D11" s="23">
-        <v>44445</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="33">
+        <v>44443</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
+      <c r="F11" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="22"/>
       <c r="B12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="13">
+        <v>44448</v>
+      </c>
+      <c r="D12" s="33">
+        <v>44444</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="22"/>
+      <c r="B13" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C12" s="13">
-        <v>44449</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
-      <c r="B13" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C13" s="13">
         <v>44449</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
+      <c r="D13" s="33">
+        <v>44445</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="22"/>
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="13">
         <v>44449</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
+      <c r="D14" s="33">
+        <v>44446</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="22"/>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="13">
         <v>44449</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
+      <c r="D15" s="33">
+        <v>44447</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="13">
         <v>44449</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
+      <c r="D16" s="33">
+        <v>44448</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="22"/>
       <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="13">
+        <v>44449</v>
+      </c>
+      <c r="D17" s="33">
+        <v>44449</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="22"/>
+      <c r="B18" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C17" s="13">
-        <v>44456</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="C18" s="13">
         <v>44456</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
+      <c r="D18" s="33">
+        <v>44450</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="13">
         <v>44456</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="17"/>
+      <c r="D19" s="33">
+        <v>44451</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="13">
         <v>44456</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
+      <c r="D20" s="33">
+        <v>44452</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="13">
         <v>44456</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="18" t="s">
+      <c r="D21" s="33">
+        <v>44453</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="22"/>
+      <c r="B22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="13">
+        <v>44456</v>
+      </c>
+      <c r="D22" s="33">
+        <v>44454</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C22" s="14">
-        <v>44463</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="18"/>
-      <c r="B23" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="C23" s="14">
         <v>44463</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="18"/>
+      <c r="D23" s="33">
+        <v>44455</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="23"/>
       <c r="B24" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="14">
         <v>44463</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="18"/>
+      <c r="D24" s="33">
+        <v>44456</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="23"/>
       <c r="B25" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="14">
         <v>44463</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="19"/>
-      <c r="B26" s="9" t="s">
+      <c r="D25" s="33">
+        <v>44457</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="23"/>
+      <c r="B26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="14">
+        <v>44463</v>
+      </c>
+      <c r="D26" s="33">
+        <v>44458</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="24"/>
+      <c r="B27" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C27" s="15">
         <v>44463</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="10"/>
+      <c r="D27" s="33">
+        <v>44459</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A10:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A10:A22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A1:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:E3">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
Revert "backlog nae changes"
This reverts commit 114e4cf645d836d2296316387394557b8317c9f5.
</commit_message>
<xml_diff>
--- a/PIP-Backlog.xlsx
+++ b/PIP-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\PIP-University-Administration-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E92157-3239-4791-B21C-E82EC84A7816}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5BB639-9238-451A-BBF7-5A4CECAD51F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18450" windowHeight="11020" xr2:uid="{59053253-4EAC-46A3-8F35-147C6248C68F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>PIP Sprint</t>
   </si>
@@ -151,12 +151,6 @@
   </si>
   <si>
     <t>Pending</t>
-  </si>
-  <si>
-    <t>UX</t>
-  </si>
-  <si>
-    <t>Design</t>
   </si>
 </sst>
 </file>
@@ -449,48 +443,48 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -818,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EF25C4-0706-4711-8224-01EE9F63F796}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -836,22 +830,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -874,7 +868,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -894,7 +888,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
@@ -912,7 +906,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -930,7 +924,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
@@ -948,7 +942,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -966,7 +960,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -984,7 +978,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1004,7 +998,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
@@ -1022,7 +1016,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
@@ -1040,7 +1034,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1048,7 @@
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1062,7 @@
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +1076,7 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="25"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1100,7 +1094,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1118,7 +1112,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1132,7 +1126,7 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1140,7 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1154,7 @@
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1174,7 +1168,7 @@
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1188,7 +1182,7 @@
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1197,81 +1191,67 @@
       <c r="C23" s="14">
         <v>44463</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23" t="s">
+      <c r="D23" s="32"/>
+      <c r="E23" s="33" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="14">
         <v>44463</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23" t="s">
+      <c r="D24" s="32"/>
+      <c r="E24" s="33" t="s">
         <v>38</v>
       </c>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="26"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="14">
         <v>44463</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23" t="s">
+      <c r="D25" s="32"/>
+      <c r="E25" s="33" t="s">
         <v>38</v>
       </c>
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="14">
         <v>44463</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23" t="s">
+      <c r="D26" s="32"/>
+      <c r="E26" s="33" t="s">
         <v>38</v>
       </c>
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="27"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="15">
-        <v>44554</v>
-      </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23" t="s">
+        <v>44463</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33" t="s">
         <v>38</v>
       </c>
       <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="15">
-        <v>44464</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Relationship & Foreign Key Update | Trials with secondary tables
</commit_message>
<xml_diff>
--- a/PIP-Backlog.xlsx
+++ b/PIP-Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\PIP-University-Administration-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5BB639-9238-451A-BBF7-5A4CECAD51F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04795BB-6017-4CE8-B343-773FB8A5281B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18450" windowHeight="11020" xr2:uid="{59053253-4EAC-46A3-8F35-147C6248C68F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18440" windowHeight="11020" xr2:uid="{59053253-4EAC-46A3-8F35-147C6248C68F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,6 +443,12 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -479,12 +485,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EF25C4-0706-4711-8224-01EE9F63F796}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:E27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,22 +830,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -868,7 +868,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -888,7 +888,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
@@ -906,7 +906,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -924,7 +924,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
@@ -942,7 +942,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -960,7 +960,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -978,7 +978,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1034,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1062,7 @@
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1094,7 +1094,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1168,7 +1168,7 @@
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1191,64 +1191,64 @@
       <c r="C23" s="14">
         <v>44463</v>
       </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33" t="s">
+      <c r="D23" s="22"/>
+      <c r="E23" s="23" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="24"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="14">
         <v>44463</v>
       </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33" t="s">
+      <c r="D24" s="22"/>
+      <c r="E24" s="23" t="s">
         <v>38</v>
       </c>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="24"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="14">
         <v>44463</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33" t="s">
+      <c r="D25" s="22"/>
+      <c r="E25" s="23" t="s">
         <v>38</v>
       </c>
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="24"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="14">
         <v>44463</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33" t="s">
+      <c r="D26" s="22"/>
+      <c r="E26" s="23" t="s">
         <v>38</v>
       </c>
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="25"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="15">
         <v>44463</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="22"/>
+      <c r="E27" s="23" t="s">
         <v>38</v>
       </c>
       <c r="F27" s="10"/>

</xml_diff>

<commit_message>
File Handling Complete: to CSV | to XLSX
</commit_message>
<xml_diff>
--- a/PIP-Backlog.xlsx
+++ b/PIP-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\PIP-University-Administration-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2135ACB8-5206-4AF9-8542-7741EBB28100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81260F-817C-4B25-A862-237C4DAF1E6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18220" windowHeight="10800" xr2:uid="{59053253-4EAC-46A3-8F35-147C6248C68F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>PIP Sprint</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Finishes</t>
+  </si>
+  <si>
+    <t>OnTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delayed </t>
   </si>
 </sst>
 </file>
@@ -814,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EF25C4-0706-4711-8224-01EE9F63F796}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1041,11 +1050,15 @@
       <c r="C13" s="13">
         <v>44449</v>
       </c>
-      <c r="D13" s="21"/>
+      <c r="D13" s="21">
+        <v>44456</v>
+      </c>
       <c r="E13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="25"/>
@@ -1055,11 +1068,15 @@
       <c r="C14" s="13">
         <v>44449</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="21">
+        <v>44456</v>
+      </c>
       <c r="E14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="25"/>
@@ -1069,11 +1086,15 @@
       <c r="C15" s="13">
         <v>44449</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="21">
+        <v>44456</v>
+      </c>
       <c r="E15" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="25"/>
@@ -1147,11 +1168,15 @@
       <c r="C20" s="13">
         <v>44456</v>
       </c>
-      <c r="D20" s="21"/>
+      <c r="D20" s="21">
+        <v>44456</v>
+      </c>
       <c r="E20" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="25"/>
@@ -1167,7 +1192,9 @@
       <c r="E21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="25"/>

</xml_diff>